<commit_message>
Minor Excel Spreadsheet changes, added README
</commit_message>
<xml_diff>
--- a/Miscellaneous/IkesExcelSpreadsheets/IkesTimeCards.xlsx
+++ b/Miscellaneous/IkesExcelSpreadsheets/IkesTimeCards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Alex\myprojects\ASheriffProjects\Miscellaneous\IkesExcelSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\ASheriffProjects\Miscellaneous\IkesExcelSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821FB21E-2007-4108-A1F0-BC7C7D045CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF0247D-2FBE-491D-AE9B-A8B0E45CF0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="315" windowWidth="24690" windowHeight="14085" xr2:uid="{9C234A68-637B-4B77-BE9D-3225315D2826}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" activeTab="1" xr2:uid="{9C234A68-637B-4B77-BE9D-3225315D2826}"/>
   </bookViews>
   <sheets>
     <sheet name="Front Staff" sheetId="1" r:id="rId1"/>
@@ -88,40 +88,40 @@
     <t>Weekly Total -&gt;</t>
   </si>
   <si>
-    <t>Kollin's Time Card</t>
-  </si>
-  <si>
-    <t>Lizzie's Time Card</t>
-  </si>
-  <si>
-    <t>Anthony's Time Card</t>
-  </si>
-  <si>
-    <t>Mason's Time Card</t>
-  </si>
-  <si>
     <t>Abel's Time Card</t>
-  </si>
-  <si>
-    <t>Caesar's Time Card</t>
-  </si>
-  <si>
-    <t>Yannette's Time Card</t>
-  </si>
-  <si>
-    <t>Ana's Time Card</t>
-  </si>
-  <si>
-    <t>Daysi's Time Card</t>
-  </si>
-  <si>
-    <t>Tio's Time Card</t>
   </si>
   <si>
     <t>TEST Time Card</t>
   </si>
   <si>
     <t>Berny's Time Card</t>
+  </si>
+  <si>
+    <t>Caitlyn's Time Card</t>
+  </si>
+  <si>
+    <t>Dallas's Time Card</t>
+  </si>
+  <si>
+    <t>Evan's Time Card</t>
+  </si>
+  <si>
+    <t>Franky's Time Card</t>
+  </si>
+  <si>
+    <t>Bellas's Time Card</t>
+  </si>
+  <si>
+    <t>Carl's Time Card</t>
+  </si>
+  <si>
+    <t>Danny's Time Card</t>
+  </si>
+  <si>
+    <t>Elaine's Time Card</t>
+  </si>
+  <si>
+    <t>Frank's Time Card</t>
   </si>
 </sst>
 </file>
@@ -221,25 +221,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -661,65 +661,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3982A38-5ACC-45A1-A08F-BE8115D484CE}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:O1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13:W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="Q1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="Q1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -784,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -843,7 +843,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -906,7 +906,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -965,7 +965,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1211,36 +1211,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="I13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="Q13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="I13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="Q13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.20416666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>0.12500000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1698,18 +1698,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="U11:V11"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="I13:O13"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="Q13:W13"/>
     <mergeCell ref="U23:V23"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="U11:V11"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F9">
     <cfRule type="expression" dxfId="12" priority="9">
@@ -1749,65 +1749,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EF0123-2698-4D4A-B0A4-536FB439C9D4}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13:W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="I1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="Q1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="Q1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2295,36 +2295,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="I13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="Q13" s="10" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="I13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="Q13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>0.20555555555555555</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>0.12500000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E23" s="5" t="s">
         <v>15</v>
       </c>
@@ -2782,18 +2782,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="U11:V11"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="I13:O13"/>
     <mergeCell ref="Q13:W13"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="U23:V23"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="U11:V11"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F9">
     <cfRule type="expression" dxfId="6" priority="6">
@@ -2837,28 +2837,28 @@
       <selection activeCell="F3" sqref="F3:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>0.29166666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0.37500000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>0.37500000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>0.37500000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>0.16666666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>